<commit_message>
finished short response 1
</commit_message>
<xml_diff>
--- a/term_1/Assignment_Planner.xlsx
+++ b/term_1/Assignment_Planner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewi\Documents\GitHub\Winter_2021-2022\2021-2022\term_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewi\Documents\GitHub\UBCO_21-22\term_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF26D20-E79D-44E7-856F-6FB963D29497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BEBED3-B085-48BE-894C-EC8638DF9927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1800" windowWidth="14400" windowHeight="7495" xr2:uid="{A664FF4E-0A93-43A8-BA8C-0E92C5698EC8}"/>
   </bookViews>
@@ -873,6 +873,51 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -917,51 +962,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142951BD-74E4-471E-868A-88909E17C9B2}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1916,11 +1916,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -1992,10 +1992,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2011,8 +2011,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2026,8 +2026,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2041,8 +2041,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2056,7 +2056,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2071,7 +2071,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2086,15 +2086,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2107,11 +2107,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2122,11 +2122,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2137,7 +2137,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2152,7 +2152,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2167,7 +2167,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2182,16 +2182,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2205,10 +2205,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2220,10 +2220,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2236,11 +2236,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2255,9 +2255,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2270,9 +2270,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -2372,6 +2372,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -2379,12 +2385,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2438,11 +2438,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -2514,10 +2514,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2533,8 +2533,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2548,8 +2548,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2563,8 +2563,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2578,7 +2578,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2593,7 +2593,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2608,15 +2608,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2629,11 +2629,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2644,11 +2644,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2659,7 +2659,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2674,7 +2674,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2689,7 +2689,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2704,16 +2704,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2727,10 +2727,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2742,10 +2742,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2758,11 +2758,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2777,9 +2777,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2792,9 +2792,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -2894,6 +2894,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -2901,12 +2907,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2960,11 +2960,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -3036,10 +3036,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3055,8 +3055,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3070,8 +3070,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3085,8 +3085,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3100,7 +3100,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3115,7 +3115,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3130,15 +3130,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3151,11 +3151,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3166,11 +3166,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3181,7 +3181,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3196,7 +3196,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3211,7 +3211,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3226,16 +3226,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3249,10 +3249,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3264,10 +3264,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3280,11 +3280,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3299,9 +3299,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3314,9 +3314,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3416,6 +3416,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3423,12 +3429,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3482,11 +3482,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -3558,10 +3558,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3577,8 +3577,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3592,8 +3592,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3607,8 +3607,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3622,7 +3622,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3637,7 +3637,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3652,15 +3652,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3673,11 +3673,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3688,11 +3688,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3703,7 +3703,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3718,7 +3718,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3733,7 +3733,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3748,16 +3748,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3771,10 +3771,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3786,10 +3786,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3802,11 +3802,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3821,9 +3821,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3836,9 +3836,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3938,6 +3938,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3945,12 +3951,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4004,11 +4004,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -4080,10 +4080,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4099,8 +4099,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4114,8 +4114,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4129,8 +4129,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4144,7 +4144,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4159,7 +4159,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4174,15 +4174,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4195,11 +4195,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4210,11 +4210,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4225,7 +4225,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4240,7 +4240,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4255,7 +4255,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4270,16 +4270,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4293,10 +4293,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4308,10 +4308,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4324,11 +4324,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4343,9 +4343,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4358,9 +4358,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -4460,6 +4460,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -4467,12 +4473,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4526,11 +4526,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -4602,10 +4602,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4621,8 +4621,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4636,8 +4636,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4651,8 +4651,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4666,7 +4666,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4681,7 +4681,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4696,15 +4696,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4717,11 +4717,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4732,11 +4732,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4747,7 +4747,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4762,7 +4762,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4777,7 +4777,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4792,16 +4792,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4815,10 +4815,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4830,10 +4830,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4846,11 +4846,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4865,9 +4865,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4880,9 +4880,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -4982,6 +4982,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -4989,12 +4995,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5517,6 +5517,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -5524,12 +5530,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6048,6 +6048,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6055,12 +6061,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6579,6 +6579,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6586,12 +6592,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7101,6 +7101,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7108,12 +7114,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7167,11 +7167,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -7243,10 +7243,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7262,8 +7262,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7277,8 +7277,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7292,8 +7292,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -7307,7 +7307,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -7322,7 +7322,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -7337,15 +7337,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -7358,11 +7358,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -7373,11 +7373,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -7388,7 +7388,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -7403,7 +7403,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -7418,7 +7418,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -7433,16 +7433,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -7456,10 +7456,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -7471,10 +7471,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -7487,11 +7487,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -7506,9 +7506,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -7521,9 +7521,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -7623,6 +7623,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7630,12 +7636,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7689,11 +7689,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -7765,10 +7765,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7784,8 +7784,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7799,8 +7799,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7814,8 +7814,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -7829,7 +7829,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -7844,7 +7844,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -7859,15 +7859,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -7880,11 +7880,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -7895,11 +7895,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -7910,7 +7910,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -7925,7 +7925,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -7940,7 +7940,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -7955,16 +7955,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -7978,10 +7978,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -7993,10 +7993,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8009,11 +8009,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8028,9 +8028,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8043,9 +8043,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8145,6 +8145,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8152,12 +8158,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8211,11 +8211,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -8287,10 +8287,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -8306,8 +8306,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -8321,8 +8321,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -8336,8 +8336,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8351,7 +8351,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8366,7 +8366,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8381,15 +8381,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8402,11 +8402,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8417,11 +8417,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8432,7 +8432,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8447,7 +8447,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -8462,7 +8462,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -8477,16 +8477,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -8500,10 +8500,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -8515,10 +8515,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8531,11 +8531,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8550,9 +8550,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8565,9 +8565,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8667,6 +8667,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8674,12 +8680,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8733,11 +8733,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="114" t="s">
+      <c r="I2" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="101"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -8809,10 +8809,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="105" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -8828,8 +8828,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="121"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -8843,8 +8843,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="121"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -8858,8 +8858,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="122"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="107"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8873,7 +8873,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8888,7 +8888,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="119"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8903,15 +8903,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="126" t="s">
+      <c r="C13" s="111" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="120" t="s">
+      <c r="F13" s="105" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8924,11 +8924,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="124"/>
-      <c r="C14" s="127"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="121"/>
+      <c r="F14" s="106"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8939,11 +8939,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="124"/>
-      <c r="C15" s="128"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="107"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8954,7 +8954,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="124"/>
+      <c r="B16" s="109"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8969,7 +8969,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="124"/>
+      <c r="B17" s="109"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -8984,7 +8984,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="125"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -8999,16 +8999,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102" t="s">
+      <c r="C19" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="105" t="s">
+      <c r="D19" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="117" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -9022,10 +9022,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="100"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="103"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -9037,10 +9037,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="101"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="104"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="122"/>
+      <c r="E21" s="119"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -9053,11 +9053,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="123" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="126" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -9072,9 +9072,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="109"/>
+      <c r="C23" s="124"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="112"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -9087,9 +9087,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="110"/>
+      <c r="C24" s="125"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="113"/>
+      <c r="E24" s="128"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -9189,6 +9189,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -9196,12 +9202,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added power point slides
</commit_message>
<xml_diff>
--- a/term_1/Assignment_Planner.xlsx
+++ b/term_1/Assignment_Planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewi\Documents\UBCO_21-22\term_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7326954E-7AEE-45C9-AA32-4D033C6D6FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C91EE-869F-48B2-AAF3-AEA47A86A0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A664FF4E-0A93-43A8-BA8C-0E92C5698EC8}"/>
   </bookViews>
@@ -894,6 +894,51 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -938,51 +983,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1937,11 +1937,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -2013,10 +2013,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2032,8 +2032,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2047,8 +2047,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2062,8 +2062,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2077,7 +2077,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2092,7 +2092,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2107,15 +2107,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2128,11 +2128,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2143,11 +2143,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2158,7 +2158,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2173,7 +2173,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2188,7 +2188,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2203,16 +2203,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2226,10 +2226,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2241,10 +2241,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2257,11 +2257,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2276,9 +2276,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2291,9 +2291,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -2393,12 +2393,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -2406,6 +2400,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2459,11 +2459,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -2535,10 +2535,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2554,8 +2554,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2569,8 +2569,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2584,8 +2584,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2599,7 +2599,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2614,7 +2614,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2629,15 +2629,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2650,11 +2650,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2665,11 +2665,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2680,7 +2680,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2695,7 +2695,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2710,7 +2710,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2725,16 +2725,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2748,10 +2748,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2763,10 +2763,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2779,11 +2779,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2798,9 +2798,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2813,9 +2813,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -2915,12 +2915,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -2928,6 +2922,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2981,11 +2981,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -3057,10 +3057,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3076,8 +3076,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3091,8 +3091,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3106,8 +3106,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3121,7 +3121,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3136,7 +3136,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3151,15 +3151,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3172,11 +3172,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3187,11 +3187,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3202,7 +3202,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3217,7 +3217,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3232,7 +3232,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3247,16 +3247,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3270,10 +3270,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3285,10 +3285,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3301,11 +3301,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3320,9 +3320,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3335,9 +3335,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3437,12 +3437,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3450,6 +3444,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3503,11 +3503,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -3579,10 +3579,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3598,8 +3598,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3613,8 +3613,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3628,8 +3628,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3643,7 +3643,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3658,7 +3658,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3673,15 +3673,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3694,11 +3694,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3709,11 +3709,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3724,7 +3724,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3739,7 +3739,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3754,7 +3754,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3769,16 +3769,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3792,10 +3792,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3807,10 +3807,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3823,11 +3823,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3842,9 +3842,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3857,9 +3857,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3959,12 +3959,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3972,6 +3966,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4025,11 +4025,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -4101,10 +4101,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4120,8 +4120,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4135,8 +4135,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4150,8 +4150,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4165,7 +4165,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4180,7 +4180,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4195,15 +4195,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4216,11 +4216,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4231,11 +4231,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4246,7 +4246,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4261,7 +4261,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4276,7 +4276,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4291,16 +4291,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4314,10 +4314,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4329,10 +4329,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4345,11 +4345,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4364,9 +4364,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4379,9 +4379,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -4481,12 +4481,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -4494,6 +4488,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4547,11 +4547,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -4623,10 +4623,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4642,8 +4642,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4657,8 +4657,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4672,8 +4672,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4687,7 +4687,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4702,7 +4702,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4717,15 +4717,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4738,11 +4738,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4753,11 +4753,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4768,7 +4768,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4783,7 +4783,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4798,7 +4798,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4813,16 +4813,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4836,10 +4836,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4851,10 +4851,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4867,11 +4867,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4886,9 +4886,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4901,9 +4901,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -5003,12 +5003,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -5016,6 +5010,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5538,12 +5538,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -5551,6 +5545,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6069,12 +6069,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6082,6 +6076,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6600,12 +6600,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6613,6 +6607,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7122,12 +7122,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7135,6 +7129,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7188,11 +7188,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -7264,10 +7264,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7283,8 +7283,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7298,8 +7298,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7313,8 +7313,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -7328,7 +7328,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -7343,7 +7343,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -7358,15 +7358,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -7379,11 +7379,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -7394,11 +7394,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -7409,7 +7409,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -7424,7 +7424,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -7439,7 +7439,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -7454,16 +7454,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -7477,10 +7477,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -7492,10 +7492,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -7508,11 +7508,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -7527,9 +7527,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -7542,9 +7542,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -7644,12 +7644,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7657,6 +7651,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7710,11 +7710,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -7786,10 +7786,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7805,8 +7805,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7820,8 +7820,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7835,8 +7835,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -7850,7 +7850,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -7865,7 +7865,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -7880,15 +7880,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -7901,11 +7901,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -7916,11 +7916,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -7931,7 +7931,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -7946,7 +7946,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -7961,7 +7961,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -7976,16 +7976,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -7999,10 +7999,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -8014,10 +8014,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8030,11 +8030,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8049,9 +8049,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8064,9 +8064,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8166,12 +8166,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8179,6 +8173,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8232,11 +8232,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -8308,10 +8308,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -8327,8 +8327,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -8342,8 +8342,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -8357,8 +8357,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8372,7 +8372,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8387,7 +8387,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8402,15 +8402,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8423,11 +8423,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8438,11 +8438,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8453,7 +8453,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8468,7 +8468,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -8483,7 +8483,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -8498,16 +8498,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -8521,10 +8521,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -8536,10 +8536,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8552,11 +8552,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8571,9 +8571,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8586,9 +8586,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8688,12 +8688,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8701,6 +8695,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8754,11 +8754,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="106"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
@@ -8830,10 +8830,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="125" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -8849,8 +8849,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="111"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="126"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -8864,8 +8864,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="111"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -8879,8 +8879,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="112"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="127"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8894,7 +8894,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="123"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8909,7 +8909,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="109"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8924,15 +8924,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="131" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="125" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8945,11 +8945,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="117"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="111"/>
+      <c r="F14" s="126"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8960,11 +8960,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="118"/>
+      <c r="B15" s="129"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="112"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8975,7 +8975,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8990,7 +8990,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="114"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -9005,7 +9005,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="115"/>
+      <c r="B18" s="130"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -9020,16 +9020,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="122" t="s">
+      <c r="C19" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="D19" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="122" t="s">
+      <c r="E19" s="107" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -9043,10 +9043,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="123"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="108"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -9058,10 +9058,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="121"/>
-      <c r="C21" s="124"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="124"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="109"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -9074,11 +9074,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="128" t="s">
+      <c r="C22" s="113" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="116" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -9093,9 +9093,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="129"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -9108,9 +9108,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="130"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -9210,12 +9210,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -9223,6 +9217,12 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Work from sep-16 PM
</commit_message>
<xml_diff>
--- a/term_1/Assignment_Planner.xlsx
+++ b/term_1/Assignment_Planner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thewi\Documents\GitHub\UBCO_21-22\term_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEE5987-B189-47EF-BC9D-08FC20CE33D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD25A9-A676-4FB9-A6C6-A8EB5ACCA5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1800" windowWidth="14400" windowHeight="7495" activeTab="1" xr2:uid="{A664FF4E-0A93-43A8-BA8C-0E92C5698EC8}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" activeTab="1" xr2:uid="{A664FF4E-0A93-43A8-BA8C-0E92C5698EC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -736,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -991,6 +991,51 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1036,51 +1081,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1412,7 +1417,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1557,13 +1562,13 @@
       <c r="F6" s="48"/>
       <c r="G6" s="6"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="75" t="s">
+      <c r="I6" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="77">
+      <c r="K6" s="71">
         <v>44455</v>
       </c>
       <c r="L6" s="1"/>
@@ -2034,11 +2039,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -2110,10 +2115,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2129,8 +2134,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2144,8 +2149,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2159,8 +2164,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2174,7 +2179,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2189,7 +2194,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2204,15 +2209,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2225,11 +2230,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2240,11 +2245,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2255,7 +2260,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2270,7 +2275,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2285,7 +2290,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2300,16 +2305,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2323,10 +2328,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2338,10 +2343,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2354,11 +2359,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2373,9 +2378,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2388,9 +2393,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -2490,6 +2495,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -2497,12 +2508,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2556,11 +2561,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -2632,10 +2637,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -2651,8 +2656,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -2666,8 +2671,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -2681,8 +2686,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -2696,7 +2701,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -2711,7 +2716,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -2726,15 +2731,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -2747,11 +2752,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -2762,11 +2767,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -2777,7 +2782,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -2792,7 +2797,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -2807,7 +2812,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -2822,16 +2827,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -2845,10 +2850,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -2860,10 +2865,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -2876,11 +2881,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -2895,9 +2900,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -2910,9 +2915,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3012,6 +3017,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3019,12 +3030,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3078,11 +3083,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -3154,10 +3159,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3173,8 +3178,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3188,8 +3193,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3203,8 +3208,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3218,7 +3223,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3233,7 +3238,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3248,15 +3253,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3269,11 +3274,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3284,11 +3289,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3299,7 +3304,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3314,7 +3319,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3329,7 +3334,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3344,16 +3349,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3367,10 +3372,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3382,10 +3387,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3398,11 +3403,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3417,9 +3422,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3432,9 +3437,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -3534,6 +3539,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -3541,12 +3552,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3600,11 +3605,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -3676,10 +3681,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -3695,8 +3700,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -3710,8 +3715,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -3725,8 +3730,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -3740,7 +3745,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -3755,7 +3760,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -3770,15 +3775,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -3791,11 +3796,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -3806,11 +3811,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -3821,7 +3826,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -3836,7 +3841,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -3851,7 +3856,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -3866,16 +3871,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -3889,10 +3894,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -3904,10 +3909,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -3920,11 +3925,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -3939,9 +3944,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -3954,9 +3959,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -4056,6 +4061,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -4063,12 +4074,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4122,11 +4127,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -4198,10 +4203,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4217,8 +4222,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4232,8 +4237,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4247,8 +4252,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4262,7 +4267,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4277,7 +4282,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4292,15 +4297,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4313,11 +4318,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4328,11 +4333,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4343,7 +4348,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4358,7 +4363,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4373,7 +4378,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4388,16 +4393,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4411,10 +4416,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4426,10 +4431,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4442,11 +4447,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4461,9 +4466,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4476,9 +4481,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -4578,6 +4583,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -4585,12 +4596,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4644,11 +4649,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -4720,10 +4725,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -4739,8 +4744,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -4754,8 +4759,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -4769,8 +4774,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -4784,7 +4789,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -4799,7 +4804,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -4814,15 +4819,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -4835,11 +4840,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -4850,11 +4855,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -4865,7 +4870,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -4880,7 +4885,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -4895,7 +4900,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -4910,16 +4915,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -4933,10 +4938,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -4948,10 +4953,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -4964,11 +4969,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -4983,9 +4988,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -4998,9 +5003,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -5100,6 +5105,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -5107,12 +5118,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5122,8 +5127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B3B8CC-D153-431F-BDAD-4E080E0238A8}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -5347,13 +5352,13 @@
       <c r="F10" s="111"/>
       <c r="G10" s="6"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="146" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="81">
+      <c r="K10" s="148">
         <v>44455</v>
       </c>
     </row>
@@ -5687,6 +5692,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="D23:D25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -5700,13 +5712,6 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="D23:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6225,6 +6230,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6232,12 +6243,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6756,6 +6761,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -6763,12 +6774,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7278,6 +7283,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7285,12 +7296,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7344,11 +7349,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -7420,10 +7425,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7439,8 +7444,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7454,8 +7459,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7469,8 +7474,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -7484,7 +7489,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -7499,7 +7504,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -7514,15 +7519,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -7535,11 +7540,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -7550,11 +7555,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -7565,7 +7570,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -7580,7 +7585,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -7595,7 +7600,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -7610,16 +7615,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -7633,10 +7638,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -7648,10 +7653,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -7664,11 +7669,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -7683,9 +7688,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -7698,9 +7703,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -7800,6 +7805,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -7807,12 +7818,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7866,11 +7871,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -7942,10 +7947,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -7961,8 +7966,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -7976,8 +7981,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -7991,8 +7996,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8006,7 +8011,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8021,7 +8026,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8036,15 +8041,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8057,11 +8062,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8072,11 +8077,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8087,7 +8092,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8102,7 +8107,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -8117,7 +8122,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -8132,16 +8137,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -8155,10 +8160,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -8170,10 +8175,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8186,11 +8191,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8205,9 +8210,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8220,9 +8225,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8322,6 +8327,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8329,12 +8340,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8388,11 +8393,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -8464,10 +8469,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -8483,8 +8488,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -8498,8 +8503,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -8513,8 +8518,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -8528,7 +8533,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -8543,7 +8548,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -8558,15 +8563,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -8579,11 +8584,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -8594,11 +8599,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -8609,7 +8614,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -8624,7 +8629,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -8639,7 +8644,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -8654,16 +8659,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -8677,10 +8682,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -8692,10 +8697,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -8708,11 +8713,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -8727,9 +8732,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -8742,9 +8747,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -8844,6 +8849,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -8851,12 +8862,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8910,11 +8915,11 @@
       <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="132"/>
-      <c r="K2" s="133"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
     </row>
     <row r="3" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A3" s="12">
@@ -8986,10 +8991,10 @@
       <c r="A7" s="14">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="122" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3"/>
@@ -9005,8 +9010,8 @@
       <c r="A8" s="14">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="138"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6"/>
       <c r="F8" s="3"/>
@@ -9020,8 +9025,8 @@
       <c r="A9" s="14">
         <v>0.375</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="138"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="3"/>
@@ -9035,8 +9040,8 @@
       <c r="A10" s="14">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="139"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="3"/>
@@ -9050,7 +9055,7 @@
       <c r="A11" s="14">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B11" s="135"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6"/>
@@ -9065,7 +9070,7 @@
       <c r="A12" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="136"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="7"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
@@ -9080,15 +9085,15 @@
       <c r="A13" s="14">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="143" t="s">
+      <c r="C13" s="128" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="122" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="6"/>
@@ -9101,11 +9106,11 @@
       <c r="A14" s="14">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B14" s="141"/>
-      <c r="C14" s="144"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="138"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="6"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23"/>
@@ -9116,11 +9121,11 @@
       <c r="A15" s="14">
         <v>0.5</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="139"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="6"/>
       <c r="H15" s="15"/>
       <c r="I15" s="23"/>
@@ -9131,7 +9136,7 @@
       <c r="A16" s="14">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
@@ -9146,7 +9151,7 @@
       <c r="A17" s="14">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="126"/>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
       <c r="E17" s="6"/>
@@ -9161,7 +9166,7 @@
       <c r="A18" s="14">
         <v>0.5625</v>
       </c>
-      <c r="B18" s="142"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="7"/>
@@ -9176,16 +9181,16 @@
       <c r="A19" s="14">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="134" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="134" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
@@ -9199,10 +9204,10 @@
       <c r="A20" s="14">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="120"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="135"/>
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="15"/>
@@ -9214,10 +9219,10 @@
       <c r="A21" s="14">
         <v>0.625</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="121"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="121"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="136"/>
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="15"/>
@@ -9230,11 +9235,11 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="125" t="s">
+      <c r="C22" s="140" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="143" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="3"/>
@@ -9249,9 +9254,9 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="126"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="129"/>
+      <c r="E23" s="144"/>
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="15"/>
@@ -9264,9 +9269,9 @@
         <v>0.6875</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="127"/>
+      <c r="C24" s="142"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="130"/>
+      <c r="E24" s="145"/>
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="15"/>
@@ -9366,6 +9371,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="B7:B12"/>
@@ -9373,12 +9384,6 @@
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>